<commit_message>
updating cv, pubs, and visualizations
</commit_message>
<xml_diff>
--- a/content/portfolio/visualizations/assets/visualizaitons-data.xlsx
+++ b/content/portfolio/visualizations/assets/visualizaitons-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ethanyoung/Google Drive/research/websites/uikit-esy/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ethanyoung/Google Drive/research/websites/uikit-esy-bundle/content/portfolio/visualizations/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{530F5E99-9519-474F-BC3F-C8628AAD2F7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F4B773-15F2-054E-B3DF-D38F55CF6201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19320" xr2:uid="{0CE67825-4914-5849-8035-CE1B79DF0A3D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="90">
   <si>
     <t>file</t>
   </si>
@@ -270,6 +270,36 @@
   </si>
   <si>
     <t>featured</t>
+  </si>
+  <si>
+    <t>Child Development</t>
+  </si>
+  <si>
+    <t>Young et al., 2022</t>
+  </si>
+  <si>
+    <t>Hidden talents in context: Cognitive performance with abstract versus ecological stimuli among adversity-exposed youth.</t>
+  </si>
+  <si>
+    <t>/publications/journal/young-2022-cd-1/</t>
+  </si>
+  <si>
+    <t>plots/cd2022-figure1.jpg</t>
+  </si>
+  <si>
+    <t>plots/cd2022-figure2.jpg</t>
+  </si>
+  <si>
+    <t>plots/cd2022-figure3.jpg</t>
+  </si>
+  <si>
+    <t>Figure 1. Schematic display of the attention shifting and working memory updating tasks: (a) abstract attention shifting, (b) ecological attention shifting, (c) abstract working memory updating, and (d) ecological working memory updating</t>
+  </si>
+  <si>
+    <t>Figure 2. Visualization of multiverse attention-shifting results. Unpredictability and violence exposure multiverse analyses were confirmatory and poverty analyses were exploratory. (a) visualizes the multiverse task version × adversity interaction on abstract and ecological task versions across high (+1 SD) and low (−1 SD) adversity exposure (y-axis was reversed so that higher values = faster shifting), (b) plots p-curves associated with each interaction term, (c) plots sorted interaction β-coefficients across each arbitrary decision, (d) plots the sample sizes for each effect, and (e) is a specification grid indicating the data processing decisions associated with each effect</t>
+  </si>
+  <si>
+    <t>Figure 3. Visualization of multiverse working memory updating results. Unpredictability and Violence exposure multiverse analyses were confirmatory and poverty analyses were exploratory. (a) visualizes the multiverse task version × adversity interaction on abstract and ecological task versions across high (+1 SD) and low (−1 SD) adversity exposure, (b) plots p-curves associated with each interaction term, (c) plots sorted interaction β-coefficients across each arbitrary decision, (d) plots the sample sizes for each effect, and (e) is a specification grid indicating the data processing decisions associated with each effect. Proportions of each arbitrary decision with p-values &lt; .05 are indicated on the right side of each specification grid. Blank proportions indicate proportions = 0. Teal lines and points reflect individual multiverse effect sizes with p-values &lt; .05</t>
   </si>
 </sst>
 </file>
@@ -631,10 +661,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45C4B627-C585-B444-ADDD-542A337891BE}">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1371,6 +1401,120 @@
         <v>0</v>
       </c>
     </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I20" s="2">
+        <v>2250</v>
+      </c>
+      <c r="J20" s="2">
+        <v>1500</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L20" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E21" s="2">
+        <v>2</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21" s="2">
+        <v>1950</v>
+      </c>
+      <c r="J21" s="2">
+        <v>2175</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L21" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22" s="2">
+        <v>3</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I22" s="2">
+        <v>1950</v>
+      </c>
+      <c r="J22" s="2">
+        <v>2175</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L22" s="2">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>